<commit_message>
invoice_generator works with excel file 'fakutra_mal'
</commit_message>
<xml_diff>
--- a/faktura_generator/data/excel/info.xlsx
+++ b/faktura_generator/data/excel/info.xlsx
@@ -5,18 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anna Stray Rongve\Google Drive\Enkeltpersonsforetak\Regnskap\faktura_generator\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anna Stray Rongve\Google Drive\Enkeltpersonsforetak\Regnskap\Fakturagenerator\faktura_generator\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16231DDC-3BD6-49E4-9CCF-1060AD955E2A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5899A8C1-5CB6-40E7-8F5A-7D6D986765CD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bedrift" sheetId="1" r:id="rId1"/>
     <sheet name="Elever" sheetId="2" r:id="rId2"/>
     <sheet name="Kunder" sheetId="3" r:id="rId3"/>
-    <sheet name="Ark1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -478,8 +477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="A1:J3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -595,7 +594,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{727B97DC-F701-48D1-9122-249827B792F2}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -641,16 +640,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64F62F22-D3E4-4383-9A97-FC8BFF262268}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>